<commit_message>
Actualizacion perfiles y ejemplos
</commit_message>
<xml_diff>
--- a/StructureDefinition-NombreSocial.xlsx
+++ b/StructureDefinition-NombreSocial.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-04T17:18:33-04:00</t>
+    <t>2023-07-19T16:02:56-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Esta extensión permite agregar un nombre social al paciente</t>
+    <t>Esta extensión permite agregar un nombre social al paciente. Se define como nombre social aquel con el cual el/la paciente se reconoce a si mismo/a</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>